<commit_message>
updated: filter and multiple page scraping
</commit_message>
<xml_diff>
--- a/realme_smartphones.xlsx
+++ b/realme_smartphones.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,61 +448,691 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>realme 13 Pro 5G (Monet Gold,8GB+128GB)</t>
+          <t>realme P2 Pro 5G (Parrot Green, 512 GB)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19801</v>
+        <v>20999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>OnePlus Nord CE4 Lite 5G (Super Silver, 8GB RAM, 128GB Storage)</t>
+          <t>realme 13 Pro+ 5G (Emerald Green, 256 GB)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17998</v>
+        <v>25999</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>realme 14 Pro+ 5G (Pearl White, 12GB RAM, 256GB Storage)| 6.83" Curved AMOLED Display | 50MP Sony IMX896 OIS + 50MP Periscope Rear Cam | 6000mAh Battery | Snapdragon 7s Gen 3 Processor | 80W SUPERVOOC</t>
+          <t>realme 13 Pro+ 5G (Monet Purple, 256 GB)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>31780</v>
+        <v>25999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>realme 13 5G (Dark Purple, 8GB RAM, 256GB Storage) | Expandable Upto 2TB | Up to 18GB Dynamic RAM | 50MP AI Dual Camera | 6.72" AMOLED Display | 45W Ultra Charging | Dimensity 6300 Processor</t>
+          <t>realme P3 Ultra 5G (Glowing Lunar White, 256 GB)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>16899</v>
+        <v>26999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>OnePlus Nord CE4 Lite 5G (Ultra Orange, 8GB RAM, 256GB Storage)</t>
+          <t>realme P2 Pro 5G (Parrot Green, 128 GB)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>20998</v>
+        <v>17999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>realme NARZO 80 Pro 5G (Speed Silver,8GB+256GB) | Segment's 1st MediaTek Dimensity 7400 Chipset | 6000mAh Titan Battery + 80W Ultra Charge | 4500nits HyperGlow Esports Display | IP69 Waterproof</t>
+          <t>realme P2 Pro 5G (Parrot Green, 256 GB)</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>21498</v>
+        <v>19999</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>realme P3 Ultra 5G (Glowing Lunar White, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>25999</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>realme 13 Pro+ 5G (Monet Gold, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>26999</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>realme 14T 5G (Lightning Purple, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>17999</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>realme 13 Pro 5G (Monet Gold, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>23999</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>realme P3 Ultra 5G (Orion Red, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>25999</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>realme 13 Pro+ 5G (Monet Purple, 512 GB)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>28999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>realme GT 6 (Fluid Silver, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>29999</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>realme 14 Pro+ 5G (Pearl White, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>31999</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>realme P3 Ultra 5G (Orion Red, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>25999</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>realme 13 Pro+ 5G (Monet Purple, 512 GB)</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>28999</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>realme 14 Pro+ 5G (Pearl White, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>31999</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>realme GT 6 (Fluid Silver, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>29999</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>realme P2 Pro 5G (Eagle Grey, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>17999</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>realme P3 Pro 5G (Nebula Glow, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>21999</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>realme P3 5G (Nebula Pink, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>15999</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>realme GT 6 (Fluid Silver, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>30999</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>realme 14x 5G (Crystal Black, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>15999</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>realme 13 Pro 5G (Emerald Green, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>21999</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>realme 13 Pro+ 5G (Monet Gold, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>25999</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>realme GT 6 (Razor Green, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>30999</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>realme 14 Pro 5G (Pearl White, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>26999</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>realme 14 Pro+ 5G (Suede Grey, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>29999</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>realme 13+ 5G (Speed Green, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>26999</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>realme P3 Ultra 5G (Neptune Blue, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>25999</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>realme P1 Speed 5G (Brushed Blue, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>16999</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>realme 13 Pro+ 5G (Monet Gold, 512 GB)</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>28999</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>realme 14 Pro 5G (Jaipur Pink, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>24999</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>realme 13 Pro 5G (Monet Purple, 512 GB)</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>26999</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>realme Narzo 70 Pro 5G (Green, Glass Green, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>19490</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>realme 7 (Mist White, 64 GB)</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>17999</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>realme 14 Pro 5G (Pearl White, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>24999</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>realme 12 Pro 5G (Submarine Blue, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>19999</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>realme 14 Pro+ 5G (Suede Grey, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>31999</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>realme Narzo 70 Pro 5G (Glass Green, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>19990</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>realme GT Neo 3 (Nitro Blue, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>24449</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>realme 14 Pro Lite 5G (Glass Gold, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>21999</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>realme 13 Pro 5G (Emerald Green, 512 GB)</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>26999</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>realme 70 TURBO 5G (Turbo Green, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>19280</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>realme 14 Pro+ 5G (Pearl White, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>29999</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>realme GT 6T 5G (Fluid Silver, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>23290</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>realme P3 Pro 5G (Saturn Brown, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>21999</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>realme 14 Pro 5G (Suede Grey, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>24999</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>realme P3 Pro 5G (Saturn Brown, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>23999</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>realme P3 Ultra 5G (Glowing Lunar White, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>24999</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>realme 14T 5G (Obsidian Black, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>17999</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>realme P3 Pro 5G (Nebula Glow, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>22999</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>realme 14T 5G (Obsidian Black, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>19999</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>realme 13 Pro+ 5G (Monet Purple, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>26999</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>realme X7 Pro 5G (Fantasy, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>29999</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>realme P1 Pro 5G (Phoenix Red, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>25999</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>realme 14 Pro Lite 5G (Glass Purple, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>21999</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>realme 70 TURBO 5G (Turbo Purple, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>16290</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>realme P1 Speed 5G (Textured Titanium, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>16990</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>realme 14 Pro+ 5G (Bikaner Purple, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>29999</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>realme NARZO 70X 5G (ICE BLUE, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>16999</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>realme 14T 5G (Lightning Purple, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>19999</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>realme 12 Pro+ 5G (Submarine Blue, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>23999</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>realme P3 Pro 5G (Saturn Brown, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>22999</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>realme 70 TURBO 5G (Turbo Yellow, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>15289</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>realme 10 Pro+ 5G (Nebula Blue, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>27999</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>realme 11 Pro 5G (Sunrise Beige, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>24999</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>realme 14 Pro 5G (Suede Grey, 256 GB)</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>26999</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>realme 10 Pro+ 5G (Nebula Blue, 128 GB)</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>25999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>